<commit_message>
Corrected bugs in lit data
- Corrected some bugs i nthe literature data file
- Fixes Figure S1 with new literature data
</commit_message>
<xml_diff>
--- a/data/Technology/LitData.xlsx
+++ b/data/Technology/LitData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\EMF33\data\Technology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76485CD-7BCC-4D06-BE22-1875E9C21B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566BD22F-943A-4611-9D53-15DCE1FC4213}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="180">
   <si>
     <t>Fuel Prices for IEA Levelized costs for electricity - 2015</t>
   </si>
@@ -632,6 +632,9 @@
   </si>
   <si>
     <t>1st gen. ethanol</t>
+  </si>
+  <si>
+    <t>LiquidsBiomassOtherwCCS</t>
   </si>
 </sst>
 </file>
@@ -2605,7 +2608,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4179,7 +4184,7 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="B52" t="s">
         <v>125</v>

</xml_diff>

<commit_message>
Added some extra outputs for Steve Rose
</commit_message>
<xml_diff>
--- a/data/Technology/LitData.xlsx
+++ b/data/Technology/LitData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\EMF33\data\Technology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566BD22F-943A-4611-9D53-15DCE1FC4213}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB9482B-2F1F-47AF-A9FD-E2FAD9100743}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="3330" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primary" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1701,8 +1703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M57"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="M49" sqref="M49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2608,9 +2610,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Corrected error in GEA data, previously used annual data
</commit_message>
<xml_diff>
--- a/data/Technology/LitData.xlsx
+++ b/data/Technology/LitData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\EMF33\data\Technology\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\User\daioglouv\Projects - Documents\EMF33\Publications\Technologies\TechData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB9482B-2F1F-47AF-A9FD-E2FAD9100743}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EC5787-1727-4E7F-8E42-EF663F8CA0F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,6 +31,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +44,7 @@
     <author>Daioglou, Vassilis</author>
   </authors>
   <commentList>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{E0E47D77-E2B1-4E1C-BA16-81CECB2AA09F}">
+    <comment ref="I7" authorId="0" shapeId="0" xr:uid="{E0E47D77-E2B1-4E1C-BA16-81CECB2AA09F}">
       <text>
         <r>
           <rPr>
@@ -68,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="H47" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="604" uniqueCount="190">
   <si>
     <t>Fuel Prices for IEA Levelized costs for electricity - 2015</t>
   </si>
@@ -234,9 +235,6 @@
     <t>Emission Factors (table 3)</t>
   </si>
   <si>
-    <t>Costs of Electricity technologies</t>
-  </si>
-  <si>
     <t>Source:</t>
   </si>
   <si>
@@ -261,9 +259,6 @@
     <t>Biomass CCS (IGCC)</t>
   </si>
   <si>
-    <t>Capital Cost [$(2010)/kW/yr]</t>
-  </si>
-  <si>
     <t>Fixed OM [$(2010)/kW/yr]</t>
   </si>
   <si>
@@ -273,9 +268,6 @@
     <t>Efficiency</t>
   </si>
   <si>
-    <t>Capital Cost [$(2005)/kW/yr]</t>
-  </si>
-  <si>
     <t>OM [$(2005)/GJ]</t>
   </si>
   <si>
@@ -597,18 +589,9 @@
     <t>CO2 Disposal [$(2007)/GJ(LHV)]</t>
   </si>
   <si>
-    <t>Capital Cost [$(2007)/GJ(LHV)]</t>
-  </si>
-  <si>
     <t>Fixed OM [$(2007)/GJ(LHV)]</t>
   </si>
   <si>
-    <t>Total Capex[$(2005)/GJ(LHV)]</t>
-  </si>
-  <si>
-    <t>Total Capex[$(2005)/kW/yr(LHV)]</t>
-  </si>
-  <si>
     <t>Capacity Factor</t>
   </si>
   <si>
@@ -636,14 +619,62 @@
     <t>1st gen. ethanol</t>
   </si>
   <si>
-    <t>LiquidsBiomassOtherwCCS</t>
+    <t>NEW</t>
+  </si>
+  <si>
+    <t>Capital Cost [$(2005)/kW-in]</t>
+  </si>
+  <si>
+    <t>kW-in</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>Interest (equation 2)</t>
+  </si>
+  <si>
+    <t>Lifetime</t>
+  </si>
+  <si>
+    <t>$(2005)/kW-out/yr</t>
+  </si>
+  <si>
+    <t>FT diesel</t>
+  </si>
+  <si>
+    <t>Capital Cost [$(2005)/kW]</t>
+  </si>
+  <si>
+    <t>Capital Cost [$(2010)/kW]</t>
+  </si>
+  <si>
+    <t>$(2005)/kW-out</t>
+  </si>
+  <si>
+    <t>Capital Cost [$(2007)]</t>
+  </si>
+  <si>
+    <t>Total Capex[$(2005)/kW]</t>
+  </si>
+  <si>
+    <t>Output [MW]</t>
+  </si>
+  <si>
+    <t>Capital Cost [$(2013)/kW]</t>
+  </si>
+  <si>
+    <t>DOUBLE CHECKING OF TECHNOLOGY DATA AFTER QUESTION FROM MARKUS MILLINGER. LARSON CALCULATION WAS WRONG!</t>
+  </si>
+  <si>
+    <t>see: Y:\User\daioglouv\Projects - Documents\EMF33\Publications\Technologies\Submission\Communications</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -738,8 +769,16 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -752,8 +791,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -907,12 +952,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -970,6 +1054,25 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -986,6 +1089,215 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5A46E3C-F554-43AD-8B3E-2D080474A0D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="20262957">
+          <a:off x="3381375" y="9648825"/>
+          <a:ext cx="2505075" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="4000" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>NOT USED</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9204432C-1ADF-4CE1-900B-219A52F70D74}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="20262957">
+          <a:off x="5934075" y="9610725"/>
+          <a:ext cx="2505075" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="4000" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>NOT USED</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="TextBox 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C09E750-A441-41E2-B4B7-4A6968D3E181}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="20262957">
+          <a:off x="8553450" y="9601200"/>
+          <a:ext cx="2505075" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="nl-NL" sz="4000" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>NOT USED</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1701,10 +2013,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M57"/>
+  <dimension ref="A2:M72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1714,895 +2026,1244 @@
     <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
     <col min="7" max="8" width="16.5703125" customWidth="1"/>
     <col min="9" max="9" width="23.42578125" customWidth="1"/>
     <col min="10" max="10" width="12" style="36" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="36"/>
+    <col min="11" max="11" width="14.5703125" style="36" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="57" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+    </row>
+    <row r="6" spans="1:11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-    </row>
-    <row r="4" spans="1:11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="B6" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="C6" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="37" t="s">
+        <v>182</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="H6" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" s="42" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>54</v>
-      </c>
-      <c r="G4" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="42" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5">
+      <c r="B7">
         <v>0.25</v>
       </c>
-      <c r="C5" s="41">
-        <f>F5*(1+$J$6)</f>
+      <c r="C7" s="55">
+        <f>F7*(1+$J$8)</f>
         <v>3584</v>
       </c>
-      <c r="D5" s="41">
-        <f t="shared" ref="D5:E8" si="0">G5*(1+$J$6)</f>
+      <c r="D7" s="41">
+        <f t="shared" ref="D7:E10" si="0">G7*(1+$J$8)</f>
         <v>85.12</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E7" s="41">
         <f t="shared" si="0"/>
         <v>8.9600000000000009</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F7" s="38">
         <v>4000</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G7" s="38">
         <v>95</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H7" s="38">
         <v>10</v>
       </c>
-      <c r="I5" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="J5" s="36" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6">
+      <c r="I7" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="J7" s="36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8">
         <v>0.18</v>
       </c>
-      <c r="C6" s="41">
-        <f t="shared" ref="C6:C8" si="1">F6*(1+$J$6)</f>
+      <c r="C8" s="55">
+        <f t="shared" ref="C8:C10" si="1">F8*(1+$J$8)</f>
         <v>6899.2</v>
       </c>
-      <c r="D6" s="41">
+      <c r="D8" s="41">
         <f t="shared" si="0"/>
         <v>103.93600000000001</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E8" s="41">
         <f t="shared" si="0"/>
         <v>12.006400000000001</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F8" s="38">
         <v>7700</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G8" s="38">
         <v>116</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H8" s="38">
         <v>13.4</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="J6" s="40">
+      <c r="I8" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="J8" s="40">
         <v>-0.104</v>
       </c>
-      <c r="K6" s="36" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7">
+      <c r="K8" s="36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9">
         <v>0.3</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C9" s="55">
         <f t="shared" si="1"/>
         <v>5376</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D9" s="41">
         <f t="shared" si="0"/>
         <v>125.44</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E9" s="41">
         <f t="shared" si="0"/>
         <v>13.44</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F9" s="38">
         <v>6000</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G9" s="38">
         <v>140</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H9" s="38">
         <v>15</v>
       </c>
-      <c r="I7" s="5" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8">
+      <c r="I9" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10">
         <v>0.25</v>
       </c>
-      <c r="C8" s="41">
+      <c r="C10" s="56">
         <f t="shared" si="1"/>
         <v>7929.6</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D10" s="41">
         <f t="shared" si="0"/>
         <v>152.32</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E10" s="41">
         <f t="shared" si="0"/>
         <v>16.128</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F10" s="38">
         <v>8850</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G10" s="38">
         <v>170</v>
       </c>
-      <c r="H8" s="38">
+      <c r="H10" s="38">
         <v>18</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I10" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15">
+        <v>0.42</v>
+      </c>
+      <c r="C15" s="50">
+        <v>1860</v>
+      </c>
+      <c r="D15">
+        <v>3.95</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16">
+        <v>0.31</v>
+      </c>
+      <c r="C16" s="51">
+        <v>2560</v>
+      </c>
+      <c r="D16">
+        <v>5.66</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21">
+        <v>0.27</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21">
+        <v>85</v>
+      </c>
+      <c r="E21">
+        <v>0.04</v>
+      </c>
+      <c r="F21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22">
+        <v>0.45</v>
+      </c>
+      <c r="C22" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>181</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="F24" s="27" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28">
+        <v>42</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29">
+        <v>35</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="F29">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="31"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="B33" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="D33" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="E33" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="F33" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="G33" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="H33" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+    </row>
+    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="D34" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="E34" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="F34" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="G34" s="47" t="s">
+        <v>177</v>
+      </c>
+      <c r="H34" s="47" t="s">
+        <v>178</v>
+      </c>
+      <c r="I34" s="47" t="s">
+        <v>176</v>
+      </c>
+      <c r="J34" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="K34" s="52" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="B35" s="46">
+        <v>0.59</v>
+      </c>
+      <c r="C35" s="46">
+        <v>394</v>
+      </c>
+      <c r="D35" s="46">
+        <v>2000</v>
+      </c>
+      <c r="E35" s="46">
+        <v>16</v>
+      </c>
+      <c r="F35" s="46">
+        <v>0.47</v>
+      </c>
+      <c r="G35" s="46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H35" s="46">
+        <v>20</v>
+      </c>
+      <c r="I35" s="46">
+        <f>G35/(1-(1+G35)^-H35)</f>
+        <v>9.4392925743255696E-2</v>
+      </c>
+      <c r="J35" s="46">
+        <f>(C35*I35)/B35</f>
+        <v>63.035275835326686</v>
+      </c>
+      <c r="K35" s="53">
+        <f>C35/B35</f>
+        <v>667.7966101694916</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="B36" s="46">
+        <v>0.59</v>
+      </c>
+      <c r="C36" s="46">
+        <v>552</v>
+      </c>
+      <c r="D36" s="46">
+        <v>400</v>
+      </c>
+      <c r="E36" s="46">
+        <v>22</v>
+      </c>
+      <c r="F36" s="46">
+        <v>0.47</v>
+      </c>
+      <c r="G36" s="46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H36" s="46">
+        <v>20</v>
+      </c>
+      <c r="I36" s="46">
+        <f>G36/(1-(1+G36)^-H36)</f>
+        <v>9.4392925743255696E-2</v>
+      </c>
+      <c r="J36" s="46">
+        <f>(C36*I36)/B36</f>
+        <v>88.313381373351106</v>
+      </c>
+      <c r="K36" s="53">
+        <f t="shared" ref="K36:K41" si="2">C36/B36</f>
+        <v>935.59322033898309</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="46">
+        <v>0.32</v>
+      </c>
+      <c r="C37" s="46">
+        <v>550</v>
+      </c>
+      <c r="D37" s="46">
+        <v>440</v>
+      </c>
+      <c r="E37" s="46">
+        <v>32</v>
+      </c>
+      <c r="F37" s="46">
+        <v>0.69</v>
+      </c>
+      <c r="G37" s="46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H37" s="46">
+        <v>20</v>
+      </c>
+      <c r="I37" s="46">
+        <f t="shared" ref="I37:I38" si="3">G37/(1-(1+G37)^-H37)</f>
+        <v>9.4392925743255696E-2</v>
+      </c>
+      <c r="J37" s="46">
+        <f t="shared" ref="J37:J38" si="4">(C37*I37)/B37</f>
+        <v>162.23784112122073</v>
+      </c>
+      <c r="K37" s="53">
+        <f t="shared" si="2"/>
+        <v>1718.75</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="B38" s="46">
+        <v>0.4</v>
+      </c>
+      <c r="C38" s="46">
+        <v>420</v>
+      </c>
+      <c r="D38" s="46">
+        <v>747</v>
+      </c>
+      <c r="E38" s="46">
+        <v>33</v>
+      </c>
+      <c r="F38" s="46">
+        <v>0.17</v>
+      </c>
+      <c r="G38" s="46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H38" s="46">
+        <v>20</v>
+      </c>
+      <c r="I38" s="46">
+        <f t="shared" si="3"/>
+        <v>9.4392925743255696E-2</v>
+      </c>
+      <c r="J38" s="46">
+        <f t="shared" si="4"/>
+        <v>99.112572030418463</v>
+      </c>
+      <c r="K38" s="53">
+        <f t="shared" si="2"/>
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" s="46">
+        <v>0.4</v>
+      </c>
+      <c r="C39" s="46">
+        <v>510</v>
+      </c>
+      <c r="D39" s="46">
+        <v>374</v>
+      </c>
+      <c r="E39" s="46">
+        <v>25</v>
+      </c>
+      <c r="F39" s="46">
+        <v>0.17</v>
+      </c>
+      <c r="G39" s="46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H39" s="46">
+        <v>20</v>
+      </c>
+      <c r="I39" s="46">
+        <f t="shared" ref="I39" si="5">G39/(1-(1+G39)^-H39)</f>
+        <v>9.4392925743255696E-2</v>
+      </c>
+      <c r="J39" s="46">
+        <f t="shared" ref="J39" si="6">(C39*I39)/B39</f>
+        <v>120.350980322651</v>
+      </c>
+      <c r="K39" s="53">
+        <f t="shared" si="2"/>
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="B40" s="46">
+        <v>0.42</v>
+      </c>
+      <c r="C40" s="46">
+        <v>539</v>
+      </c>
+      <c r="D40" s="46">
+        <v>2000</v>
+      </c>
+      <c r="E40" s="46">
+        <v>30</v>
+      </c>
+      <c r="F40" s="46">
+        <v>0</v>
+      </c>
+      <c r="G40" s="46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H40" s="46">
+        <v>20</v>
+      </c>
+      <c r="I40" s="46">
+        <f t="shared" ref="I40" si="7">G40/(1-(1+G40)^-H40)</f>
+        <v>9.4392925743255696E-2</v>
+      </c>
+      <c r="J40" s="46">
+        <f t="shared" ref="J40" si="8">(C40*I40)/B40</f>
+        <v>121.13758803717815</v>
+      </c>
+      <c r="K40" s="53">
+        <f t="shared" si="2"/>
+        <v>1283.3333333333335</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="48" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" s="46">
+        <v>0.42</v>
+      </c>
+      <c r="C41" s="46">
+        <v>686</v>
+      </c>
+      <c r="D41" s="46">
+        <v>400</v>
+      </c>
+      <c r="E41" s="46">
+        <v>24</v>
+      </c>
+      <c r="F41" s="46">
+        <v>0</v>
+      </c>
+      <c r="G41" s="46">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H41" s="46">
+        <v>20</v>
+      </c>
+      <c r="I41" s="46">
+        <f t="shared" ref="I41" si="9">G41/(1-(1+G41)^-H41)</f>
+        <v>9.4392925743255696E-2</v>
+      </c>
+      <c r="J41" s="46">
+        <f t="shared" ref="J41" si="10">(C41*I41)/B41</f>
+        <v>154.17511204731764</v>
+      </c>
+      <c r="K41" s="54">
+        <f t="shared" si="2"/>
+        <v>1633.3333333333335</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="31"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="31"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="35"/>
+      <c r="D46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="35"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+    </row>
+    <row r="47" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D47" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="E47" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G47" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="H47" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="I47" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="J47" s="30"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="32"/>
+      <c r="D48">
+        <v>63.36</v>
+      </c>
+      <c r="F48" t="s">
+        <v>90</v>
+      </c>
+      <c r="G48">
+        <v>0.8</v>
+      </c>
+      <c r="H48">
+        <v>30</v>
+      </c>
+      <c r="I48">
+        <v>121.02</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C49" s="32"/>
+      <c r="D49">
+        <v>4</v>
+      </c>
+      <c r="F49" t="s">
+        <v>94</v>
+      </c>
+      <c r="G49">
+        <v>0.8</v>
+      </c>
+      <c r="H49">
+        <v>30</v>
+      </c>
+      <c r="I49">
+        <v>7.06</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="32"/>
+      <c r="D50">
+        <v>41.22</v>
+      </c>
+      <c r="F50" t="s">
+        <v>95</v>
+      </c>
+      <c r="G50">
+        <v>0.75</v>
+      </c>
+      <c r="H50">
+        <v>30</v>
+      </c>
+      <c r="I50">
+        <v>56.83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="32"/>
+      <c r="D51">
+        <v>52.13</v>
+      </c>
+      <c r="F51" t="s">
+        <v>95</v>
+      </c>
+      <c r="G51">
+        <v>0.48</v>
+      </c>
+      <c r="H51">
+        <v>30</v>
+      </c>
+      <c r="I51">
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="32"/>
+      <c r="D52">
+        <v>60.52</v>
+      </c>
+      <c r="F52" t="s">
+        <v>95</v>
+      </c>
+      <c r="G52">
+        <v>0.48</v>
+      </c>
+      <c r="H52">
+        <v>30</v>
+      </c>
+      <c r="I52">
+        <v>76.19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" s="32"/>
+      <c r="D53">
+        <v>21.1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>96</v>
+      </c>
+      <c r="G53">
+        <v>0.65</v>
+      </c>
+      <c r="H53">
+        <v>30</v>
+      </c>
+      <c r="I53">
+        <v>11.52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="32"/>
+      <c r="D54">
+        <v>14.46</v>
+      </c>
+      <c r="F54" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54">
+        <v>0.85</v>
+      </c>
+      <c r="H54">
+        <v>30</v>
+      </c>
+      <c r="I54">
+        <v>53.16</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A57" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="35"/>
+      <c r="F57" s="35"/>
+      <c r="G57" s="35"/>
+      <c r="H57" s="35"/>
+      <c r="I57" s="35"/>
+    </row>
+    <row r="59" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C59" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="E59" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="F59" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="G59" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="H59" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="I59" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="J59" s="37" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" s="51">
+        <f>(J60*(1+L61))</f>
+        <v>3509.5439999999999</v>
+      </c>
+      <c r="D60">
+        <v>107.2</v>
+      </c>
+      <c r="E60">
+        <v>5.34</v>
+      </c>
+      <c r="F60" t="s">
+        <v>147</v>
+      </c>
+      <c r="G60">
+        <v>8.7799999999999994</v>
+      </c>
+      <c r="H60">
+        <v>2.5732104757215537</v>
+      </c>
+      <c r="I60">
+        <v>0.38861958997722101</v>
+      </c>
+      <c r="J60" s="38">
+        <v>4188</v>
+      </c>
+      <c r="L60" s="36" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L61" s="40">
+        <v>-0.16200000000000001</v>
+      </c>
+      <c r="M61" s="36" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A63" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="B63" s="35" t="s">
+        <v>157</v>
+      </c>
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="35"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="35"/>
+      <c r="I63" s="35"/>
+    </row>
+    <row r="65" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B65" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C65" s="26" t="s">
+        <v>184</v>
+      </c>
+      <c r="D65" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="E65" s="26" t="s">
+        <v>161</v>
+      </c>
+      <c r="F65" s="26" t="s">
+        <v>160</v>
+      </c>
+      <c r="G65" s="26" t="s">
+        <v>186</v>
+      </c>
+      <c r="H65" s="49" t="s">
+        <v>185</v>
+      </c>
+      <c r="I65" s="27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>158</v>
+      </c>
+      <c r="B66">
+        <v>46.5</v>
+      </c>
+      <c r="C66">
+        <v>724000000</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>-2.2599999999999998</v>
+      </c>
+      <c r="F66">
+        <f>SUM(C66:E66)</f>
+        <v>723999997.74000001</v>
+      </c>
+      <c r="G66">
+        <v>286</v>
+      </c>
+      <c r="H66" s="50">
+        <f>(C66*(1-J69))/(G66*1000)</f>
+        <v>2678.2937062937062</v>
+      </c>
+      <c r="I66">
+        <v>3.57</v>
+      </c>
+      <c r="J66" s="36" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="E12" s="27" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13">
-        <v>0.42</v>
-      </c>
-      <c r="C13">
-        <v>1860</v>
-      </c>
-      <c r="D13">
-        <v>3.95</v>
-      </c>
-      <c r="E13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14">
-        <v>0.31</v>
-      </c>
-      <c r="C14">
-        <v>2560</v>
-      </c>
-      <c r="D14">
-        <v>5.66</v>
-      </c>
-      <c r="E14">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="35"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-    </row>
-    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="27" t="s">
-        <v>65</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19">
-        <v>0.27</v>
-      </c>
-      <c r="C19" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19">
-        <v>85</v>
-      </c>
-      <c r="E19">
-        <v>0.04</v>
-      </c>
-      <c r="F19" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20">
-        <v>0.45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="27" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="33" t="s">
-        <v>74</v>
-      </c>
-      <c r="E23" t="s">
-        <v>69</v>
-      </c>
-      <c r="F23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="B24">
-        <v>49</v>
-      </c>
-      <c r="C24" t="s">
-        <v>72</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" t="s">
-        <v>77</v>
-      </c>
-      <c r="C25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="B26">
-        <v>42</v>
-      </c>
-      <c r="C26" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" t="s">
-        <v>84</v>
-      </c>
-      <c r="F26">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="B27">
-        <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>86</v>
-      </c>
-      <c r="D27" t="s">
-        <v>87</v>
-      </c>
-      <c r="F27">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="35" t="s">
-        <v>105</v>
-      </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="35"/>
-      <c r="I31" s="35"/>
-    </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="D32" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="E32" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="F32" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="G32" s="27" t="s">
-        <v>92</v>
-      </c>
-      <c r="H32" s="27" t="s">
-        <v>102</v>
-      </c>
-      <c r="I32" s="26" t="s">
+      <c r="B67">
+        <v>46.5</v>
+      </c>
+      <c r="C67">
+        <v>737000000</v>
+      </c>
+      <c r="D67">
+        <v>1.38</v>
+      </c>
+      <c r="E67">
+        <v>-1.81</v>
+      </c>
+      <c r="F67">
+        <f>SUM(C67:E67)</f>
+        <v>736999999.57000005</v>
+      </c>
+      <c r="G67">
+        <v>286</v>
+      </c>
+      <c r="H67" s="51">
+        <f>(C67*(1-J69))/(G67*1000)</f>
+        <v>2726.3846153846152</v>
+      </c>
+      <c r="I67">
+        <v>3.63</v>
+      </c>
+      <c r="J67" s="36" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J69" s="40">
+        <v>-5.8000000000000003E-2</v>
+      </c>
+      <c r="K69" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="J32" s="30"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="C33" s="32"/>
-      <c r="D33">
-        <v>63.36</v>
-      </c>
-      <c r="F33" t="s">
-        <v>93</v>
-      </c>
-      <c r="G33">
-        <v>0.8</v>
-      </c>
-      <c r="H33">
-        <v>30</v>
-      </c>
-      <c r="I33">
-        <v>121.02</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="C34" s="32"/>
-      <c r="D34">
-        <v>4</v>
-      </c>
-      <c r="F34" t="s">
-        <v>97</v>
-      </c>
-      <c r="G34">
-        <v>0.8</v>
-      </c>
-      <c r="H34">
-        <v>30</v>
-      </c>
-      <c r="I34">
-        <v>7.06</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="32"/>
-      <c r="D35">
-        <v>41.22</v>
-      </c>
-      <c r="F35" t="s">
-        <v>98</v>
-      </c>
-      <c r="G35">
-        <v>0.75</v>
-      </c>
-      <c r="H35">
-        <v>30</v>
-      </c>
-      <c r="I35">
-        <v>56.83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="C36" s="32"/>
-      <c r="D36">
-        <v>52.13</v>
-      </c>
-      <c r="F36" t="s">
-        <v>98</v>
-      </c>
-      <c r="G36">
-        <v>0.48</v>
-      </c>
-      <c r="H36">
-        <v>30</v>
-      </c>
-      <c r="I36">
-        <v>37.799999999999997</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
-        <v>96</v>
-      </c>
-      <c r="C37" s="32"/>
-      <c r="D37">
-        <v>60.52</v>
-      </c>
-      <c r="F37" t="s">
-        <v>98</v>
-      </c>
-      <c r="G37">
-        <v>0.48</v>
-      </c>
-      <c r="H37">
-        <v>30</v>
-      </c>
-      <c r="I37">
-        <v>76.19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C38" s="32"/>
-      <c r="D38">
-        <v>21.1</v>
-      </c>
-      <c r="F38" t="s">
-        <v>99</v>
-      </c>
-      <c r="G38">
-        <v>0.65</v>
-      </c>
-      <c r="H38">
-        <v>30</v>
-      </c>
-      <c r="I38">
-        <v>11.52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C39" s="32"/>
-      <c r="D39">
-        <v>14.46</v>
-      </c>
-      <c r="F39" t="s">
-        <v>6</v>
-      </c>
-      <c r="G39">
-        <v>0.85</v>
-      </c>
-      <c r="H39">
-        <v>30</v>
-      </c>
-      <c r="I39">
-        <v>53.16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="35"/>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="35"/>
-    </row>
-    <row r="44" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>58</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>100</v>
-      </c>
-      <c r="E44" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="F44" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="G44" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="H44" s="27" t="s">
-        <v>152</v>
-      </c>
-      <c r="I44" s="26" t="s">
-        <v>57</v>
-      </c>
-      <c r="J44" s="37" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>149</v>
-      </c>
-      <c r="C45">
-        <v>3509.5439999999999</v>
-      </c>
-      <c r="D45">
-        <v>107.2</v>
-      </c>
-      <c r="E45">
-        <v>5.34</v>
-      </c>
-      <c r="F45" t="s">
-        <v>150</v>
-      </c>
-      <c r="G45">
-        <v>8.7799999999999994</v>
-      </c>
-      <c r="H45">
-        <v>2.5732104757215537</v>
-      </c>
-      <c r="I45">
-        <v>0.38861958997722101</v>
-      </c>
-      <c r="J45" s="38">
-        <v>4188</v>
-      </c>
-      <c r="L45" s="36" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L46" s="40">
-        <v>-0.16200000000000001</v>
-      </c>
-      <c r="M46" s="36" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="35" t="s">
-        <v>160</v>
-      </c>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="35"/>
-      <c r="G48" s="35"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="35"/>
-    </row>
-    <row r="50" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="B50" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="D50" s="26" t="s">
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J70" s="36">
+        <v>0.9</v>
+      </c>
+      <c r="K70" s="36" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J71" s="36">
+        <v>8760</v>
+      </c>
+      <c r="K71" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="E50" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="F50" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="G50" s="26" t="s">
-        <v>168</v>
-      </c>
-      <c r="H50" s="26" t="s">
-        <v>169</v>
-      </c>
-      <c r="I50" s="27" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>161</v>
-      </c>
-      <c r="B51">
-        <v>46.5</v>
-      </c>
-      <c r="C51">
-        <v>13.77</v>
-      </c>
-      <c r="D51">
-        <v>0</v>
-      </c>
-      <c r="E51">
-        <v>-2.2599999999999998</v>
-      </c>
-      <c r="F51">
-        <f>SUM(C51:E51)</f>
-        <v>11.51</v>
-      </c>
-      <c r="G51">
-        <f>F51*(1+$J$54)</f>
-        <v>10.842419999999999</v>
-      </c>
-      <c r="H51">
-        <f>G51*$J$57*$J$55*$J$56*(1/1000)</f>
-        <v>307.73390140800001</v>
-      </c>
-      <c r="I51">
-        <v>3.57</v>
-      </c>
-      <c r="J51" s="36" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>162</v>
-      </c>
-      <c r="B52">
-        <v>46.5</v>
-      </c>
-      <c r="C52">
-        <v>14</v>
-      </c>
-      <c r="D52">
-        <v>1.38</v>
-      </c>
-      <c r="E52">
-        <v>-1.81</v>
-      </c>
-      <c r="F52">
-        <f>SUM(C52:E52)</f>
-        <v>13.569999999999999</v>
-      </c>
-      <c r="G52">
-        <f>F52*(1+$J$54)</f>
-        <v>12.782939999999998</v>
-      </c>
-      <c r="H52">
-        <f>G52*$J$57*$J$55*$J$56*(1/1000)</f>
-        <v>362.81051625599997</v>
-      </c>
-      <c r="I52">
-        <v>3.63</v>
-      </c>
-      <c r="J52" s="36" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J54" s="40">
-        <v>-5.8000000000000003E-2</v>
-      </c>
-      <c r="K54" s="43" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J55" s="36">
-        <v>0.9</v>
-      </c>
-      <c r="K55" s="36" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J56" s="36">
-        <v>8760</v>
-      </c>
-      <c r="K56" s="36" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J57" s="36">
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J72" s="36">
         <v>3.6</v>
       </c>
-      <c r="K57" s="36" t="s">
+      <c r="K72" s="36" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K54" r:id="rId1" xr:uid="{F17D9F7A-6123-460E-9A12-A39907B7B95D}"/>
+    <hyperlink ref="K69" r:id="rId1" xr:uid="{F17D9F7A-6123-460E-9A12-A39907B7B95D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <customProperties>
     <customPr name="EpmWorksheetKeyString_GUID" r:id="rId3"/>
   </customProperties>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2610,7 +3271,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2624,51 +3287,51 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
         <v>108</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" t="s">
-        <v>109</v>
-      </c>
-      <c r="D1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>112</v>
       </c>
-      <c r="F1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" t="s">
-        <v>177</v>
-      </c>
-      <c r="H1" t="s">
-        <v>113</v>
-      </c>
-      <c r="I1" t="s">
-        <v>115</v>
-      </c>
       <c r="J1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C2" t="s">
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F2">
         <v>0.39</v>
@@ -2677,27 +3340,27 @@
         <v>3509.5</v>
       </c>
       <c r="I2" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="J2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C3" t="s">
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F3">
         <v>0.25</v>
@@ -2706,27 +3369,27 @@
         <v>3584</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
         <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F4">
         <v>0.18</v>
@@ -2735,27 +3398,27 @@
         <v>6899.2</v>
       </c>
       <c r="I4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F5">
         <v>0.3</v>
@@ -2764,27 +3427,27 @@
         <v>5376</v>
       </c>
       <c r="I5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F6">
         <v>0.25</v>
@@ -2793,27 +3456,27 @@
         <v>7929.6</v>
       </c>
       <c r="I6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="J6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F7">
         <v>0.42</v>
@@ -2822,27 +3485,27 @@
         <v>1860</v>
       </c>
       <c r="I7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F8">
         <v>0.31</v>
@@ -2851,27 +3514,27 @@
         <v>2560</v>
       </c>
       <c r="I8" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F9">
         <v>0.27</v>
@@ -2880,27 +3543,27 @@
         <v>2600</v>
       </c>
       <c r="I9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F10">
         <v>0.27</v>
@@ -2909,79 +3572,79 @@
         <v>4100</v>
       </c>
       <c r="I10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H11">
         <v>1850</v>
       </c>
       <c r="I11" t="s">
+        <v>116</v>
+      </c>
+      <c r="J11" t="s">
         <v>119</v>
-      </c>
-      <c r="J11" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H12">
         <v>2800</v>
       </c>
       <c r="I12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J12" t="s">
         <v>119</v>
-      </c>
-      <c r="J12" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E13" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F13">
         <v>0.45</v>
@@ -2990,27 +3653,27 @@
         <v>1900</v>
       </c>
       <c r="I13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J13" t="s">
         <v>119</v>
-      </c>
-      <c r="J13" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E14" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F14">
         <v>0.45</v>
@@ -3019,27 +3682,27 @@
         <v>3500</v>
       </c>
       <c r="I14" t="s">
+        <v>116</v>
+      </c>
+      <c r="J14" t="s">
         <v>119</v>
-      </c>
-      <c r="J14" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E15" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F15">
         <v>0.45</v>
@@ -3048,27 +3711,27 @@
         <v>1200</v>
       </c>
       <c r="I15" t="s">
+        <v>116</v>
+      </c>
+      <c r="J15" t="s">
         <v>119</v>
-      </c>
-      <c r="J15" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E16" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F16">
         <v>0.45</v>
@@ -3077,27 +3740,27 @@
         <v>2200</v>
       </c>
       <c r="I16" t="s">
+        <v>116</v>
+      </c>
+      <c r="J16" t="s">
         <v>119</v>
-      </c>
-      <c r="J16" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E17" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F17">
         <v>0.36</v>
@@ -3106,27 +3769,27 @@
         <v>430</v>
       </c>
       <c r="I17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J17" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B18" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E18" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F18">
         <v>0.36</v>
@@ -3135,27 +3798,27 @@
         <v>500</v>
       </c>
       <c r="I18" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J18" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B19" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E19" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F19">
         <v>0.52</v>
@@ -3167,27 +3830,27 @@
         <v>498.07692307692304</v>
       </c>
       <c r="I19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J19" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F20">
         <v>0.52</v>
@@ -3199,27 +3862,27 @@
         <v>688.46153846153845</v>
       </c>
       <c r="I20" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C21" t="s">
         <v>38</v>
       </c>
       <c r="D21" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E21" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F21">
         <v>0.54</v>
@@ -3231,27 +3894,27 @@
         <v>446.29629629629625</v>
       </c>
       <c r="I21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B22" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C22" t="s">
         <v>38</v>
       </c>
       <c r="D22" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E22" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F22">
         <v>0.54</v>
@@ -3263,27 +3926,27 @@
         <v>574.07407407407402</v>
       </c>
       <c r="I22" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J22" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C23" t="s">
         <v>38</v>
       </c>
       <c r="D23" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F23">
         <v>0.62</v>
@@ -3295,27 +3958,27 @@
         <v>254.83870967741936</v>
       </c>
       <c r="I23" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C24" t="s">
         <v>38</v>
       </c>
       <c r="D24" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E24" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F24">
         <v>0.62</v>
@@ -3327,27 +3990,27 @@
         <v>327.41935483870969</v>
       </c>
       <c r="I24" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J24" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B25" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C25" t="s">
         <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E25" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F25">
         <v>0.49</v>
@@ -3359,27 +4022,27 @@
         <v>448.9795918367347</v>
       </c>
       <c r="I25" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J25" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B26" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E26" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F26">
         <v>0.49</v>
@@ -3391,27 +4054,27 @@
         <v>575.51020408163265</v>
       </c>
       <c r="I26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J26" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C27" t="s">
         <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E27" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F27">
         <v>0.54</v>
@@ -3423,27 +4086,27 @@
         <v>775.92592592592587</v>
       </c>
       <c r="I27" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J27" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B28" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
       </c>
       <c r="D28" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E28" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F28">
         <v>0.54</v>
@@ -3455,27 +4118,27 @@
         <v>1022.2222222222222</v>
       </c>
       <c r="I28" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J28" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B29" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
       </c>
       <c r="D29" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E29" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F29">
         <v>0.53</v>
@@ -3487,27 +4150,27 @@
         <v>271.69811320754718</v>
       </c>
       <c r="I29" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J29" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B30" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C30" t="s">
         <v>38</v>
       </c>
       <c r="D30" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="E30" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F30">
         <v>0.53</v>
@@ -3519,27 +4182,27 @@
         <v>349.05660377358487</v>
       </c>
       <c r="I30" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B31" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C31" t="s">
         <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E31" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F31">
         <v>0.49</v>
@@ -3551,27 +4214,27 @@
         <v>289.79591836734693</v>
       </c>
       <c r="I31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C32" t="s">
         <v>38</v>
       </c>
       <c r="D32" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E32" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F32">
         <v>0.49</v>
@@ -3583,27 +4246,27 @@
         <v>340.81632653061223</v>
       </c>
       <c r="I32" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J32" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C33" t="s">
         <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E33" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F33">
         <v>0.92</v>
@@ -3615,27 +4278,27 @@
         <v>53.260869565217391</v>
       </c>
       <c r="I33" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J33" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C34" t="s">
         <v>38</v>
       </c>
       <c r="D34" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E34" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F34">
         <v>0.92</v>
@@ -3647,27 +4310,27 @@
         <v>72.826086956521735</v>
       </c>
       <c r="I34" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J34" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C35" t="s">
         <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E35" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F35">
         <v>0.37</v>
@@ -3679,27 +4342,27 @@
         <v>1343.2432432432433</v>
       </c>
       <c r="I35" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J35" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B36" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C36" t="s">
         <v>38</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E36" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F36">
         <v>0.35</v>
@@ -3711,27 +4374,27 @@
         <v>1508.5714285714287</v>
       </c>
       <c r="I36" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J36" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B37" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
       </c>
       <c r="D37" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E37" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F37">
         <v>0.35</v>
@@ -3743,27 +4406,27 @@
         <v>1951.4285714285716</v>
       </c>
       <c r="I37" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J37" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B38" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C38" t="s">
         <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E38" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F38">
         <v>0.44</v>
@@ -3775,27 +4438,27 @@
         <v>1277.2727272727273</v>
       </c>
       <c r="I38" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J38" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B39" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C39" t="s">
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E39" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F39">
         <v>0.44</v>
@@ -3807,27 +4470,27 @@
         <v>1068.1818181818182</v>
       </c>
       <c r="I39" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J39" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B40" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C40" t="s">
         <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E40" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F40">
         <v>0.32</v>
@@ -3839,27 +4502,27 @@
         <v>1718.75</v>
       </c>
       <c r="I40" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J40" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B41" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C41" t="s">
         <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E41" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F41">
         <v>0.4</v>
@@ -3871,27 +4534,27 @@
         <v>1050</v>
       </c>
       <c r="I41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J41" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B42" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C42" t="s">
         <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E42" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F42">
         <v>0.4</v>
@@ -3903,27 +4566,27 @@
         <v>1275</v>
       </c>
       <c r="I42" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J42" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B43" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C43" t="s">
         <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E43" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F43">
         <v>0.59</v>
@@ -3935,27 +4598,27 @@
         <v>667.7966101694916</v>
       </c>
       <c r="I43" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J43" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B44" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C44" t="s">
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E44" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F44">
         <v>0.59</v>
@@ -3967,27 +4630,27 @@
         <v>935.59322033898309</v>
       </c>
       <c r="I44" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J44" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B45" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C45" t="s">
         <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E45" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F45">
         <v>0.42</v>
@@ -3999,27 +4662,27 @@
         <v>1283.3333333333335</v>
       </c>
       <c r="I45" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J45" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B46" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C46" t="s">
         <v>38</v>
       </c>
       <c r="D46" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E46" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F46">
         <v>0.42</v>
@@ -4031,27 +4694,27 @@
         <v>1633.3333333333335</v>
       </c>
       <c r="I46" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J46" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B47" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C47" t="s">
         <v>38</v>
       </c>
       <c r="D47" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E47" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F47">
         <v>0.35</v>
@@ -4063,27 +4726,27 @@
         <v>1220</v>
       </c>
       <c r="I47" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J47" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B48" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C48" t="s">
         <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E48" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F48">
         <v>0.35</v>
@@ -4095,120 +4758,120 @@
         <v>1657.1428571428573</v>
       </c>
       <c r="I48" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J48" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B49" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C49" t="s">
         <v>38</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E49" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H49">
         <v>420</v>
       </c>
       <c r="I49" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J49" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B50" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C50" t="s">
         <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E50" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="H50">
         <v>600</v>
       </c>
       <c r="I50" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="J50" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B51" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C51" t="s">
         <v>38</v>
       </c>
       <c r="D51" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E51" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F51">
         <v>0.46500000000000002</v>
       </c>
       <c r="H51">
-        <v>307.73390140800001</v>
+        <v>2678.2937062937062</v>
       </c>
       <c r="I51" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="J51" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>179</v>
+        <v>133</v>
       </c>
       <c r="B52" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C52" t="s">
         <v>38</v>
       </c>
       <c r="D52" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E52" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F52">
         <v>0.46500000000000002</v>
       </c>
       <c r="H52">
-        <v>362.81051625599997</v>
+        <v>2726.3846153846152</v>
       </c>
       <c r="I52" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="J52" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>